<commit_message>
Added data for a few more pesticides as well as a stacked bar graph plot to visualize the proportion of each compound per WHO toxicity classification group
</commit_message>
<xml_diff>
--- a/ToxicologyProject/data/NIH_Toxicology.xlsx
+++ b/ToxicologyProject/data/NIH_Toxicology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heaton\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30061FC3-96E5-4225-AD5E-31125C466C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AB689C-65C1-43D0-A225-1BB141C8A36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6765" windowWidth="29040" windowHeight="16440" xr2:uid="{530E84CD-69A8-48DF-AD71-204925FC4024}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{530E84CD-69A8-48DF-AD71-204925FC4024}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,8 @@
   <authors>
     <author>tc={685C6D05-5276-41E4-A596-B0B9EDC789F5}</author>
     <author>tc={AD78B316-4165-4794-97AA-D7A6B9A89B51}</author>
+    <author>tc={6C5EF388-DAB9-428D-9016-A704C79EBEC7}</author>
+    <author>tc={02CB797C-27E0-4B42-96C3-A444C5713C3A}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{685C6D05-5276-41E4-A596-B0B9EDC789F5}">
@@ -57,12 +59,30 @@
 Additional Remark: Petroleum is not used as a pesticide by itself.</t>
       </text>
     </comment>
+    <comment ref="D11" authorId="2" shapeId="0" xr:uid="{6C5EF388-DAB9-428D-9016-A704C79EBEC7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Could be incorrect</t>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="3" shapeId="0" xr:uid="{02CB797C-27E0-4B42-96C3-A444C5713C3A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://pubchem.ncbi.nlm.nih.gov/compound/5971#section=Toxicological-Information
+Reply:
+    What to do if multiple reported LD50? Just average?</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Pesticide/Compound</t>
   </si>
@@ -104,13 +124,34 @@
   </si>
   <si>
     <t>AnnualUseKG</t>
+  </si>
+  <si>
+    <t>Sulfuric Acid</t>
+  </si>
+  <si>
+    <t>Propanil</t>
+  </si>
+  <si>
+    <t>Copper Sulfate Tribasic</t>
+  </si>
+  <si>
+    <t>Chloropicrin</t>
+  </si>
+  <si>
+    <t>Methyl Bromide (Bromomethane)</t>
+  </si>
+  <si>
+    <t>Cyanamide</t>
+  </si>
+  <si>
+    <t>Allyl Isothiocyanate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +171,12 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -485,20 +532,29 @@
     <text>Remark: Don't feel comfortable using this value. Petroleum is a mixture of hydrocarbons and each... mixture has a slightly different composition. It is very difficult to find LD50/LC50 values for Petroleum since pesticides that use petroleum as an ingredient do not publish the exact proportions.
 Additional Remark: Petroleum is not used as a pesticide by itself.</text>
   </threadedComment>
+  <threadedComment ref="D11" dT="2022-11-21T02:44:20.09" personId="{2F1DE12B-0F4A-4FB8-BD0D-EE774F89A4E7}" id="{6C5EF388-DAB9-428D-9016-A704C79EBEC7}">
+    <text>Could be incorrect</text>
+  </threadedComment>
+  <threadedComment ref="A17" dT="2022-11-21T02:57:39.43" personId="{2F1DE12B-0F4A-4FB8-BD0D-EE774F89A4E7}" id="{02CB797C-27E0-4B42-96C3-A444C5713C3A}">
+    <text>https://pubchem.ncbi.nlm.nih.gov/compound/5971#section=Toxicological-Information</text>
+  </threadedComment>
+  <threadedComment ref="A17" dT="2022-11-21T02:57:59.53" personId="{2F1DE12B-0F4A-4FB8-BD0D-EE774F89A4E7}" id="{D805635A-22E3-43A6-BACC-612C0630EE3C}" parentId="{02CB797C-27E0-4B42-96C3-A444C5713C3A}">
+    <text>What to do if multiple reported LD50? Just average?</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35E7AA3-D019-4B00-BC13-FBF17E6516EB}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -634,14 +690,112 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>347</v>
+      <c r="B10" t="s">
+        <v>11</v>
       </c>
       <c r="C10">
         <v>375</v>
       </c>
       <c r="D10">
         <v>21489465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>2140</v>
+      </c>
+      <c r="D11">
+        <v>34014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>2500</v>
+      </c>
+      <c r="D12">
+        <v>20584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>367</v>
+      </c>
+      <c r="D13">
+        <v>18083</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>250</v>
+      </c>
+      <c r="D14">
+        <v>12923</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>214</v>
+      </c>
+      <c r="D15">
+        <v>10742</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>388</v>
+      </c>
+      <c r="C16">
+        <v>125</v>
+      </c>
+      <c r="D16">
+        <v>9178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>308</v>
+      </c>
+      <c r="C17">
+        <v>148</v>
+      </c>
+      <c r="D17">
+        <v>8908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data for a few more pesticides and added visuals to be used during Monday's meeting
</commit_message>
<xml_diff>
--- a/ToxicologyProject/data/NIH_Toxicology.xlsx
+++ b/ToxicologyProject/data/NIH_Toxicology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heaton\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30061FC3-96E5-4225-AD5E-31125C466C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AB689C-65C1-43D0-A225-1BB141C8A36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6765" windowWidth="29040" windowHeight="16440" xr2:uid="{530E84CD-69A8-48DF-AD71-204925FC4024}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{530E84CD-69A8-48DF-AD71-204925FC4024}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,8 @@
   <authors>
     <author>tc={685C6D05-5276-41E4-A596-B0B9EDC789F5}</author>
     <author>tc={AD78B316-4165-4794-97AA-D7A6B9A89B51}</author>
+    <author>tc={6C5EF388-DAB9-428D-9016-A704C79EBEC7}</author>
+    <author>tc={02CB797C-27E0-4B42-96C3-A444C5713C3A}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{685C6D05-5276-41E4-A596-B0B9EDC789F5}">
@@ -57,12 +59,30 @@
 Additional Remark: Petroleum is not used as a pesticide by itself.</t>
       </text>
     </comment>
+    <comment ref="D11" authorId="2" shapeId="0" xr:uid="{6C5EF388-DAB9-428D-9016-A704C79EBEC7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Could be incorrect</t>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="3" shapeId="0" xr:uid="{02CB797C-27E0-4B42-96C3-A444C5713C3A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    https://pubchem.ncbi.nlm.nih.gov/compound/5971#section=Toxicological-Information
+Reply:
+    What to do if multiple reported LD50? Just average?</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Pesticide/Compound</t>
   </si>
@@ -104,13 +124,34 @@
   </si>
   <si>
     <t>AnnualUseKG</t>
+  </si>
+  <si>
+    <t>Sulfuric Acid</t>
+  </si>
+  <si>
+    <t>Propanil</t>
+  </si>
+  <si>
+    <t>Copper Sulfate Tribasic</t>
+  </si>
+  <si>
+    <t>Chloropicrin</t>
+  </si>
+  <si>
+    <t>Methyl Bromide (Bromomethane)</t>
+  </si>
+  <si>
+    <t>Cyanamide</t>
+  </si>
+  <si>
+    <t>Allyl Isothiocyanate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +171,12 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -485,20 +532,29 @@
     <text>Remark: Don't feel comfortable using this value. Petroleum is a mixture of hydrocarbons and each... mixture has a slightly different composition. It is very difficult to find LD50/LC50 values for Petroleum since pesticides that use petroleum as an ingredient do not publish the exact proportions.
 Additional Remark: Petroleum is not used as a pesticide by itself.</text>
   </threadedComment>
+  <threadedComment ref="D11" dT="2022-11-21T02:44:20.09" personId="{2F1DE12B-0F4A-4FB8-BD0D-EE774F89A4E7}" id="{6C5EF388-DAB9-428D-9016-A704C79EBEC7}">
+    <text>Could be incorrect</text>
+  </threadedComment>
+  <threadedComment ref="A17" dT="2022-11-21T02:57:39.43" personId="{2F1DE12B-0F4A-4FB8-BD0D-EE774F89A4E7}" id="{02CB797C-27E0-4B42-96C3-A444C5713C3A}">
+    <text>https://pubchem.ncbi.nlm.nih.gov/compound/5971#section=Toxicological-Information</text>
+  </threadedComment>
+  <threadedComment ref="A17" dT="2022-11-21T02:57:59.53" personId="{2F1DE12B-0F4A-4FB8-BD0D-EE774F89A4E7}" id="{D805635A-22E3-43A6-BACC-612C0630EE3C}" parentId="{02CB797C-27E0-4B42-96C3-A444C5713C3A}">
+    <text>What to do if multiple reported LD50? Just average?</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35E7AA3-D019-4B00-BC13-FBF17E6516EB}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -634,14 +690,112 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>347</v>
+      <c r="B10" t="s">
+        <v>11</v>
       </c>
       <c r="C10">
         <v>375</v>
       </c>
       <c r="D10">
         <v>21489465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>2140</v>
+      </c>
+      <c r="D11">
+        <v>34014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>2500</v>
+      </c>
+      <c r="D12">
+        <v>20584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>367</v>
+      </c>
+      <c r="D13">
+        <v>18083</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>250</v>
+      </c>
+      <c r="D14">
+        <v>12923</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>214</v>
+      </c>
+      <c r="D15">
+        <v>10742</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>388</v>
+      </c>
+      <c r="C16">
+        <v>125</v>
+      </c>
+      <c r="D16">
+        <v>9178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>308</v>
+      </c>
+      <c r="C17">
+        <v>148</v>
+      </c>
+      <c r="D17">
+        <v>8908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>